<commit_message>
J05AR -> XX1 correction
Thanks Yann!
</commit_message>
<xml_diff>
--- a/data-raw/IeDEA_druglist.xlsx
+++ b/data-raw/IeDEA_druglist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C971EF-FCCC-42C7-B67D-115D2665CB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45F5719-3AB9-4E7B-B08A-337B198CB628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1187,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2334,8 +2334,8 @@
       <c r="D57" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>66</v>
+      <c r="E57" s="5" t="s">
+        <v>264</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>131</v>

</xml_diff>

<commit_message>
Entecavir -> ETC, Riplivirine -> RPV
</commit_message>
<xml_diff>
--- a/data-raw/IeDEA_druglist.xlsx
+++ b/data-raw/IeDEA_druglist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45F5719-3AB9-4E7B-B08A-337B198CB628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFD496B-228E-4E48-944B-96D5B07105E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="269">
   <si>
     <t>J05A</t>
   </si>
@@ -760,9 +760,6 @@
     <t>AZT D4T NVP</t>
   </si>
   <si>
-    <t xml:space="preserve">ETV FTC TDF </t>
-  </si>
-  <si>
     <t xml:space="preserve">EFV EVG TDF </t>
   </si>
   <si>
@@ -833,6 +830,12 @@
   </si>
   <si>
     <t>XX4</t>
+  </si>
+  <si>
+    <t>ETC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FTC RPV TDF </t>
   </si>
 </sst>
 </file>
@@ -1187,21 +1190,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="16.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -1221,7 +1224,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
@@ -1241,7 +1244,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1255,13 +1258,13 @@
         <v>66</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>177</v>
       </c>
@@ -1275,13 +1278,13 @@
         <v>227</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1295,13 +1298,13 @@
         <v>67</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1321,7 +1324,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>181</v>
       </c>
@@ -1361,7 +1364,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1421,7 +1424,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>183</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1461,7 +1464,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1501,7 +1504,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>82</v>
       </c>
@@ -1541,7 +1544,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>172</v>
       </c>
@@ -1561,7 +1564,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1601,7 +1604,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>179</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -1641,7 +1644,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>186</v>
       </c>
@@ -1655,13 +1658,13 @@
         <v>66</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1681,7 +1684,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -1701,7 +1704,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -1721,7 +1724,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>28</v>
       </c>
@@ -1741,7 +1744,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -1761,7 +1764,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -1781,12 +1784,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>56</v>
@@ -1801,7 +1804,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>198</v>
       </c>
@@ -1815,13 +1818,13 @@
         <v>227</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
@@ -1841,7 +1844,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1854,14 +1857,14 @@
       <c r="D33" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>93</v>
+      <c r="E33" s="5" t="s">
+        <v>267</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>200</v>
       </c>
@@ -1881,27 +1884,27 @@
         <v>227</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>248</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>188</v>
       </c>
@@ -1921,7 +1924,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>190</v>
       </c>
@@ -1941,7 +1944,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>192</v>
       </c>
@@ -1955,13 +1958,13 @@
         <v>227</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>194</v>
       </c>
@@ -1981,7 +1984,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>196</v>
       </c>
@@ -2001,7 +2004,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>202</v>
       </c>
@@ -2015,13 +2018,13 @@
         <v>227</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>38</v>
       </c>
@@ -2041,7 +2044,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>39</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>41</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>99</v>
       </c>
@@ -2121,7 +2124,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>135</v>
       </c>
@@ -2135,13 +2138,13 @@
         <v>93</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>136</v>
       </c>
@@ -2155,13 +2158,13 @@
         <v>93</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>204</v>
       </c>
@@ -2181,7 +2184,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>206</v>
       </c>
@@ -2201,7 +2204,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>208</v>
       </c>
@@ -2221,7 +2224,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>210</v>
       </c>
@@ -2241,7 +2244,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>133</v>
       </c>
@@ -2261,7 +2264,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>45</v>
       </c>
@@ -2281,7 +2284,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>230</v>
       </c>
@@ -2301,7 +2304,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>47</v>
       </c>
@@ -2315,13 +2318,13 @@
         <v>66</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>49</v>
       </c>
@@ -2335,13 +2338,13 @@
         <v>66</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>100</v>
       </c>
@@ -2361,7 +2364,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>173</v>
       </c>
@@ -2381,7 +2384,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>174</v>
       </c>
@@ -2401,7 +2404,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>217</v>
       </c>
@@ -2409,7 +2412,7 @@
         <v>218</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>238</v>
@@ -2421,7 +2424,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>103</v>
       </c>
@@ -2441,7 +2444,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>107</v>
       </c>
@@ -2461,7 +2464,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>137</v>
       </c>
@@ -2481,7 +2484,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>138</v>
       </c>
@@ -2494,14 +2497,14 @@
       <c r="D65" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>243</v>
+      <c r="E65" s="5" t="s">
+        <v>268</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>139</v>
       </c>
@@ -2515,13 +2518,13 @@
         <v>161</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>109</v>
       </c>
@@ -2541,7 +2544,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>140</v>
       </c>
@@ -2555,13 +2558,13 @@
         <v>165</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>141</v>
       </c>
@@ -2581,7 +2584,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>142</v>
       </c>
@@ -2601,7 +2604,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>143</v>
       </c>
@@ -2621,12 +2624,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>250</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>101</v>
@@ -2635,33 +2638,33 @@
         <v>227</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>231</v>
       </c>
       <c r="B73" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>253</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>254</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>232</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>221</v>
       </c>
@@ -2681,7 +2684,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>233</v>
       </c>
@@ -2689,7 +2692,7 @@
         <v>234</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>235</v>
@@ -2701,7 +2704,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>223</v>
       </c>
@@ -2715,13 +2718,13 @@
         <v>228</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>224</v>
       </c>
@@ -2729,7 +2732,7 @@
         <v>225</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>236</v>
@@ -2741,7 +2744,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>50</v>
       </c>
@@ -2761,7 +2764,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>51</v>
       </c>
@@ -2781,7 +2784,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>52</v>
       </c>
@@ -2801,7 +2804,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>151</v>
       </c>
@@ -2821,7 +2824,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>122</v>
       </c>
@@ -2841,7 +2844,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>154</v>
       </c>
@@ -2861,7 +2864,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>152</v>
       </c>
@@ -2881,7 +2884,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>53</v>
       </c>
@@ -2901,7 +2904,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>54</v>
       </c>
@@ -2921,7 +2924,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="87" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>156</v>
       </c>

</xml_diff>

<commit_message>
Raltegravir & Elvitegravir fixes #2
</commit_message>
<xml_diff>
--- a/data-raw/IeDEA_druglist.xlsx
+++ b/data-raw/IeDEA_druglist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B437D9-CDFD-45CF-AC96-CEA1CA9A11F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD87436-B18C-486C-AC00-41029098F72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="754" yWindow="754" windowWidth="24686" windowHeight="13149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="275">
   <si>
     <t>J05A</t>
   </si>
@@ -839,6 +839,21 @@
   </si>
   <si>
     <t>MOZ</t>
+  </si>
+  <si>
+    <t>J05AJ01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raltegravir </t>
+  </si>
+  <si>
+    <t>RAL</t>
+  </si>
+  <si>
+    <t>J05AJ02</t>
+  </si>
+  <si>
+    <t>Elvitegravir</t>
   </si>
 </sst>
 </file>
@@ -1191,23 +1206,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="16.53515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="47.3046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.69140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.84375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.84375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -1227,7 +1242,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
@@ -1247,7 +1262,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1267,7 +1282,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>177</v>
       </c>
@@ -1287,7 +1302,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1307,7 +1322,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1327,7 +1342,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1347,7 +1362,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>181</v>
       </c>
@@ -1367,7 +1382,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1387,7 +1402,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1407,7 +1422,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1427,7 +1442,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>183</v>
       </c>
@@ -1447,7 +1462,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1467,7 +1482,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1487,7 +1502,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1507,7 +1522,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1527,7 +1542,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>82</v>
       </c>
@@ -1547,7 +1562,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>172</v>
       </c>
@@ -1567,7 +1582,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1587,7 +1602,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1607,7 +1622,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>179</v>
       </c>
@@ -1627,7 +1642,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -1647,7 +1662,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>186</v>
       </c>
@@ -1667,7 +1682,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1687,7 +1702,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -1707,7 +1722,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -1727,7 +1742,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>28</v>
       </c>
@@ -1747,7 +1762,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -1767,7 +1782,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -1787,7 +1802,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -1807,7 +1822,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>198</v>
       </c>
@@ -1827,7 +1842,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
@@ -1847,7 +1862,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1867,7 +1882,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>200</v>
       </c>
@@ -1887,7 +1902,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="s">
         <v>246</v>
       </c>
@@ -1907,7 +1922,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>188</v>
       </c>
@@ -1927,7 +1942,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>190</v>
       </c>
@@ -1947,7 +1962,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>192</v>
       </c>
@@ -1967,7 +1982,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>194</v>
       </c>
@@ -1987,7 +2002,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>196</v>
       </c>
@@ -2007,7 +2022,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>202</v>
       </c>
@@ -2027,7 +2042,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>38</v>
       </c>
@@ -2047,7 +2062,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>39</v>
       </c>
@@ -2067,7 +2082,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
         <v>41</v>
       </c>
@@ -2087,7 +2102,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -2107,7 +2122,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
         <v>99</v>
       </c>
@@ -2127,7 +2142,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>135</v>
       </c>
@@ -2147,7 +2162,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>136</v>
       </c>
@@ -2167,7 +2182,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>204</v>
       </c>
@@ -2187,7 +2202,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>206</v>
       </c>
@@ -2207,7 +2222,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>208</v>
       </c>
@@ -2227,7 +2242,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>210</v>
       </c>
@@ -2247,7 +2262,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
         <v>133</v>
       </c>
@@ -2267,7 +2282,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>45</v>
       </c>
@@ -2287,669 +2302,709 @@
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A55" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A56" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A57" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A58" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E58" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A59" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E59" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A60" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>216</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>101</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>176</v>
+        <v>102</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>176</v>
+        <v>102</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>262</v>
+        <v>215</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>238</v>
+        <v>175</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>241</v>
+        <v>175</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
-        <v>103</v>
+        <v>174</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>104</v>
+        <v>216</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>106</v>
+        <v>176</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>106</v>
+        <v>176</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
-        <v>107</v>
+        <v>217</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>105</v>
+        <v>218</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>262</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>108</v>
+        <v>238</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>108</v>
+        <v>241</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>105</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>159</v>
+        <v>106</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>242</v>
+        <v>106</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>149</v>
+        <v>219</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>105</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>268</v>
+        <v>108</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>162</v>
+        <v>105</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
-        <v>109</v>
+        <v>138</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>220</v>
+        <v>149</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>163</v>
+        <v>105</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>268</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>105</v>
+        <v>162</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A70" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A72" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E72" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F72" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+    <row r="73" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E73" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F73" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+    <row r="74" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E72" s="5" t="s">
+      <c r="D74" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="F72" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="F74" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A75" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D75" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="E75" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="F73" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+      <c r="F75" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C76" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E76" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F74" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="F76" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D77" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="E77" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="F75" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+      <c r="F77" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A78" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B78" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C78" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="F76" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+      <c r="F78" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A79" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C79" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F77" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+      <c r="F79" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A80" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>111</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
-        <v>151</v>
+        <v>51</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>226</v>
+        <v>115</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>116</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>124</v>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A82" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>155</v>
+        <v>226</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>116</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A84" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A85" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A86" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D86" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="E86" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="F86" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A87" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="D87" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="E87" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="F87" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A88" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D88" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="E88" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F86" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+      <c r="F88" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="D89" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="E89" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="F89" s="2" t="s">
         <v>227</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F87">
-    <sortCondition ref="A2:A87"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F89">
+    <sortCondition ref="A2:A89"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>